<commit_message>
reorder delay rows -- need to fix hlines
</commit_message>
<xml_diff>
--- a/data/marburg/raw/marburg_parameter.xlsx
+++ b/data/marburg/raw/marburg_parameter.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc4018\Documents\code\priority-pathogens\src\data_cleaning\data\marburg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc4018\Documents\code\priority-pathogens\data\marburg\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACEB0E3-4714-4FF5-88AC-EFD2ED114C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC8DD39-4F95-4B31-B8F4-6BB21D392377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter data - Table" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Parameter data - Table'!$B$1:$B$87</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2516" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="211">
   <si>
     <t>Parameter_data_ID</t>
   </si>
@@ -492,9 +495,6 @@
   </si>
   <si>
     <t>Doubling time</t>
-  </si>
-  <si>
-    <t>2.0</t>
   </si>
   <si>
     <t>Human delay - serial interval</t>
@@ -952,7 +952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -976,11 +976,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1001,6 +1000,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1342,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO24" sqref="AO24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,16 +1574,12 @@
       <c r="E2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
       <c r="H2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
       <c r="M2" s="3" t="s">
         <v>51</v>
       </c>
@@ -1734,19 +1738,19 @@
         <v>0</v>
       </c>
       <c r="AD3" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE3" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AF3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG3" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="AF3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="AI3" s="3" t="s">
         <v>51</v>
@@ -1798,14 +1802,12 @@
       <c r="C4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="10"/>
       <c r="E4" s="3" t="s">
         <v>51</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="10"/>
       <c r="J4" s="3" t="s">
         <v>51</v>
       </c>
@@ -1874,7 +1876,6 @@
       <c r="AK4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AN4" s="10"/>
       <c r="AO4" s="6" t="s">
         <v>51</v>
       </c>
@@ -1913,10 +1914,10 @@
       <c r="B5" s="2">
         <v>21</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -2380,8 +2381,6 @@
       <c r="AK8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AL8" s="10"/>
-      <c r="AM8" s="10"/>
       <c r="AN8" s="9">
         <v>374</v>
       </c>
@@ -2432,7 +2431,7 @@
       <c r="E9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>142</v>
       </c>
       <c r="J9" s="3" t="s">
@@ -2638,8 +2637,6 @@
       <c r="AK10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AL10" s="10"/>
-      <c r="AM10" s="10"/>
       <c r="AN10" s="9">
         <v>374</v>
       </c>
@@ -2703,8 +2700,6 @@
       <c r="M11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
       <c r="P11" s="3" t="s">
         <v>51</v>
       </c>
@@ -2894,8 +2889,6 @@
       <c r="AK12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AL12" s="10"/>
-      <c r="AM12" s="10"/>
       <c r="AN12" s="4">
         <v>31</v>
       </c>
@@ -3069,7 +3062,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D14" s="9">
         <v>11</v>
@@ -3090,7 +3083,7 @@
         <v>15</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>51</v>
@@ -3152,9 +3145,6 @@
       <c r="AK14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AL14" s="10"/>
-      <c r="AM14" s="10"/>
-      <c r="AN14" s="10"/>
       <c r="AO14" s="6" t="s">
         <v>51</v>
       </c>
@@ -3194,7 +3184,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D15" s="4">
         <v>14.3</v>
@@ -3290,7 +3280,7 @@
         <v>68</v>
       </c>
       <c r="AP15" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ15" s="3" t="s">
         <v>51</v>
@@ -3342,8 +3332,6 @@
       <c r="M16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
       <c r="P16" s="3" t="s">
         <v>51</v>
       </c>
@@ -3460,16 +3448,12 @@
       <c r="E17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
       <c r="H17" s="3" t="s">
         <v>105</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
       <c r="M17" s="3" t="s">
         <v>51</v>
       </c>
@@ -3548,7 +3532,7 @@
         <v>68</v>
       </c>
       <c r="AP17" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ17" s="3" t="s">
         <v>51</v>
@@ -3844,8 +3828,6 @@
       <c r="E20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
       <c r="H20" s="3" t="s">
         <v>143</v>
       </c>
@@ -3861,8 +3843,6 @@
       <c r="M20" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
       <c r="P20" s="3" t="s">
         <v>51</v>
       </c>
@@ -3923,8 +3903,6 @@
       <c r="AK20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AL20" s="10"/>
-      <c r="AM20" s="10"/>
       <c r="AN20" s="4">
         <v>374</v>
       </c>
@@ -3992,8 +3970,6 @@
       <c r="M21" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
       <c r="P21" s="3" t="s">
         <v>51</v>
       </c>
@@ -4158,7 +4134,7 @@
         <v>0</v>
       </c>
       <c r="AD22" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AE22" s="6" t="s">
         <v>51</v>
@@ -4194,7 +4170,7 @@
         <v>68</v>
       </c>
       <c r="AP22" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ22" s="3" t="s">
         <v>51</v>
@@ -4243,7 +4219,7 @@
       <c r="G23" s="9">
         <v>30</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="14" t="s">
         <v>105</v>
       </c>
       <c r="J23" s="3" t="s">
@@ -4327,7 +4303,7 @@
         <v>68</v>
       </c>
       <c r="AP23" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ23" s="3" t="s">
         <v>51</v>
@@ -4364,23 +4340,23 @@
       <c r="C24" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="4">
-        <v>5.67</v>
+      <c r="D24" s="18">
+        <v>5.6700000000000001E-4</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="16" t="s">
         <v>51</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K24" s="9">
-        <v>0.49</v>
-      </c>
-      <c r="L24" s="9">
-        <v>8.9700000000000006</v>
+      <c r="K24" s="20">
+        <v>4.8999999999999998E-5</v>
+      </c>
+      <c r="L24" s="20">
+        <v>8.9700000000000001E-4</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>147</v>
@@ -4499,7 +4475,7 @@
       <c r="E25" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="17" t="s">
         <v>105</v>
       </c>
       <c r="J25" s="3" t="s">
@@ -4616,7 +4592,7 @@
         <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="9">
         <v>0.38</v>
@@ -4624,17 +4600,15 @@
       <c r="E26" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="16" t="s">
         <v>51</v>
       </c>
       <c r="I26" s="9">
         <v>4.6900000000000004</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
+        <v>198</v>
+      </c>
       <c r="M26" s="3" t="s">
         <v>51</v>
       </c>
@@ -4704,7 +4678,7 @@
         <v>2</v>
       </c>
       <c r="AO26" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AP26" s="7" t="s">
         <v>135</v>
@@ -4728,7 +4702,7 @@
         <v>117</v>
       </c>
       <c r="AW26" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AX26" s="5" t="b">
         <v>0</v>
@@ -4742,7 +4716,7 @@
         <v>48</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D27" s="4">
         <v>1.27</v>
@@ -4750,24 +4724,20 @@
       <c r="E27" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="17" t="s">
+      <c r="H27" s="16" t="s">
         <v>51</v>
       </c>
       <c r="I27" s="9">
         <v>2.29</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
       <c r="P27" s="3" t="s">
         <v>51</v>
       </c>
@@ -4828,13 +4798,11 @@
       <c r="AK27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AL27" s="10"/>
-      <c r="AM27" s="10"/>
       <c r="AN27" s="9">
         <v>2</v>
       </c>
       <c r="AO27" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AP27" s="7" t="s">
         <v>135</v>
@@ -4858,7 +4826,7 @@
         <v>117</v>
       </c>
       <c r="AW27" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AX27" s="5" t="b">
         <v>0</v>
@@ -4871,28 +4839,24 @@
       <c r="B28" s="2">
         <v>33</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>153</v>
+      <c r="C28" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D28" s="19">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H28" s="16" t="s">
         <v>51</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
       <c r="M28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
       <c r="P28" s="3" t="s">
         <v>51</v>
       </c>
@@ -4995,7 +4959,7 @@
         <v>48</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D29" s="4">
         <v>3.6</v>
@@ -5003,14 +4967,14 @@
       <c r="E29" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="16" t="s">
         <v>51</v>
       </c>
       <c r="I29" s="9">
         <v>2.57</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>51</v>
@@ -5083,7 +5047,7 @@
         <v>2</v>
       </c>
       <c r="AO29" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AP29" s="7" t="s">
         <v>135</v>
@@ -5107,7 +5071,7 @@
         <v>117</v>
       </c>
       <c r="AW29" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AX29" s="5" t="b">
         <v>0</v>
@@ -5121,7 +5085,7 @@
         <v>51</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D30" s="4">
         <v>3.6000000000000002E-4</v>
@@ -5129,14 +5093,14 @@
       <c r="E30" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" s="15" t="s">
         <v>143</v>
       </c>
       <c r="I30" s="9">
         <v>2.5700000000000001E-4</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
@@ -5229,7 +5193,7 @@
         <v>51</v>
       </c>
       <c r="AW30" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AX30" s="5" t="b">
         <v>0</v>
@@ -5243,7 +5207,7 @@
         <v>51</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D31" s="9">
         <v>3.8000000000000002E-5</v>
@@ -5258,7 +5222,7 @@
         <v>4.6900000000000002E-4</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>51</v>
@@ -5348,7 +5312,7 @@
         <v>51</v>
       </c>
       <c r="AW31" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AX31" s="5" t="b">
         <v>0</v>
@@ -5362,7 +5326,7 @@
         <v>51</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D32" s="9">
         <v>1.27E-4</v>
@@ -5377,7 +5341,7 @@
         <v>2.2900000000000001E-4</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M32" s="3" t="s">
         <v>51</v>
@@ -5472,7 +5436,7 @@
         <v>51</v>
       </c>
       <c r="AW32" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AX32" s="5" t="b">
         <v>0</v>
@@ -5486,7 +5450,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D33" s="4">
         <v>1.59</v>
@@ -5534,7 +5498,7 @@
         <v>80</v>
       </c>
       <c r="Z33" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA33" s="6" t="s">
         <v>51</v>
@@ -5731,7 +5695,7 @@
         <v>42</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="3" t="s">
@@ -5783,19 +5747,19 @@
         <v>0</v>
       </c>
       <c r="AD35" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AE35" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AF35" s="3" t="s">
         <v>51</v>
       </c>
       <c r="AG35" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH35" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="AH35" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="AI35" s="3" t="s">
         <v>65</v>
@@ -5819,7 +5783,7 @@
         <v>68</v>
       </c>
       <c r="AP35" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ35" s="3" t="s">
         <v>51</v>
@@ -5854,7 +5818,7 @@
         <v>43</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="3" t="s">
@@ -5871,8 +5835,6 @@
       <c r="M36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
       <c r="P36" s="3" t="s">
         <v>51</v>
       </c>
@@ -5910,19 +5872,19 @@
         <v>0</v>
       </c>
       <c r="AD36" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AE36" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF36" s="3" t="s">
         <v>51</v>
       </c>
       <c r="AG36" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH36" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="AH36" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="AI36" s="3" t="s">
         <v>65</v>
@@ -5931,7 +5893,7 @@
         <v>58</v>
       </c>
       <c r="AK36" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AN36" s="4">
         <v>102</v>
@@ -5943,7 +5905,7 @@
         <v>138</v>
       </c>
       <c r="AQ36" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AR36" s="3" t="s">
         <v>70</v>
@@ -5952,7 +5914,7 @@
         <v>140</v>
       </c>
       <c r="AT36" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AU36" s="3" t="s">
         <v>72</v>
@@ -5975,7 +5937,7 @@
         <v>43</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="3" t="s">
@@ -6029,19 +5991,19 @@
         <v>0</v>
       </c>
       <c r="AD37" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AE37" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF37" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AF37" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="AG37" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH37" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="AH37" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="AI37" s="3" t="s">
         <v>65</v>
@@ -6050,10 +6012,8 @@
         <v>58</v>
       </c>
       <c r="AK37" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AL37" s="10"/>
-      <c r="AM37" s="10"/>
+        <v>166</v>
+      </c>
       <c r="AN37" s="4">
         <v>102</v>
       </c>
@@ -6064,7 +6024,7 @@
         <v>138</v>
       </c>
       <c r="AQ37" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AR37" s="3" t="s">
         <v>70</v>
@@ -6073,7 +6033,7 @@
         <v>140</v>
       </c>
       <c r="AT37" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AU37" s="3" t="s">
         <v>72</v>
@@ -6096,7 +6056,7 @@
         <v>58</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="3" t="s">
@@ -6150,16 +6110,16 @@
         <v>0</v>
       </c>
       <c r="AD38" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AE38" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF38" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AG38" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AH38" s="3" t="s">
         <v>98</v>
@@ -6213,7 +6173,7 @@
         <v>58</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="3" t="s">
@@ -6267,16 +6227,16 @@
         <v>0</v>
       </c>
       <c r="AD39" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AE39" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AF39" s="3" t="s">
         <v>51</v>
       </c>
       <c r="AG39" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AH39" s="3" t="s">
         <v>98</v>
@@ -6648,7 +6608,7 @@
         <v>51</v>
       </c>
       <c r="AA42" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB42" s="5" t="b">
         <v>1</v>
@@ -6687,7 +6647,7 @@
         <v>94</v>
       </c>
       <c r="AP42" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AQ42" s="3" t="s">
         <v>51</v>
@@ -6998,8 +6958,6 @@
       <c r="J45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K45" s="10"/>
-      <c r="L45" s="10"/>
       <c r="M45" s="3" t="s">
         <v>51</v>
       </c>
@@ -7323,8 +7281,6 @@
       <c r="AK47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AL47" s="10"/>
-      <c r="AM47" s="10"/>
       <c r="AN47" s="9">
         <v>1899</v>
       </c>
@@ -7566,19 +7522,19 @@
         <v>0</v>
       </c>
       <c r="AD49" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE49" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="AE49" s="6" t="s">
+      <c r="AF49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG49" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AF49" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG49" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="AH49" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AI49" s="3" t="s">
         <v>65</v>
@@ -7602,7 +7558,7 @@
         <v>110</v>
       </c>
       <c r="AP49" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AQ49" s="3" t="s">
         <v>51</v>
@@ -7654,7 +7610,6 @@
       <c r="H50" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="I50" s="10"/>
       <c r="J50" s="3" t="s">
         <v>51</v>
       </c>
@@ -7695,7 +7650,7 @@
         <v>51</v>
       </c>
       <c r="AA50" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AB50" s="5" t="b">
         <v>1</v>
@@ -7737,10 +7692,10 @@
         <v>225</v>
       </c>
       <c r="AO50" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP50" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="AP50" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="AQ50" s="3" t="s">
         <v>51</v>
@@ -7749,16 +7704,16 @@
         <v>89</v>
       </c>
       <c r="AS50" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="AT50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU50" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="AT50" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU50" s="3" t="s">
+      <c r="AV50" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="AV50" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="AW50" s="7" t="s">
         <v>51</v>
@@ -7867,7 +7822,7 @@
         <v>57</v>
       </c>
       <c r="AP51" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AQ51" s="3" t="s">
         <v>51</v>
@@ -8171,8 +8126,6 @@
       <c r="M54" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="N54" s="10"/>
-      <c r="O54" s="10"/>
       <c r="P54" s="3" t="s">
         <v>51</v>
       </c>
@@ -8233,8 +8186,6 @@
       <c r="AK54" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AL54" s="10"/>
-      <c r="AM54" s="10"/>
       <c r="AN54" s="4">
         <v>121</v>
       </c>
@@ -8291,8 +8242,6 @@
       <c r="J55" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K55" s="10"/>
-      <c r="L55" s="10"/>
       <c r="M55" s="3" t="s">
         <v>51</v>
       </c>
@@ -8418,8 +8367,6 @@
       <c r="J56" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K56" s="10"/>
-      <c r="L56" s="10"/>
       <c r="M56" s="3" t="s">
         <v>51</v>
       </c>
@@ -8570,7 +8517,7 @@
         <v>51</v>
       </c>
       <c r="AA57" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AB57" s="5" t="b">
         <v>1</v>
@@ -8609,7 +8556,7 @@
         <v>94</v>
       </c>
       <c r="AP57" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AQ57" s="3" t="s">
         <v>51</v>
@@ -8618,7 +8565,7 @@
         <v>89</v>
       </c>
       <c r="AS57" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AT57" s="3" t="s">
         <v>51</v>
@@ -8627,7 +8574,7 @@
         <v>89</v>
       </c>
       <c r="AV57" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AW57" s="7" t="s">
         <v>51</v>
@@ -8743,7 +8690,7 @@
         <v>89</v>
       </c>
       <c r="AS58" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AT58" s="3" t="s">
         <v>51</v>
@@ -8752,7 +8699,7 @@
         <v>89</v>
       </c>
       <c r="AV58" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AW58" s="7" t="s">
         <v>51</v>
@@ -8861,25 +8808,25 @@
         <v>110</v>
       </c>
       <c r="AP59" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AQ59" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR59" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS59" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="AQ59" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR59" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS59" s="3" t="s">
+      <c r="AT59" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU59" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV59" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="AT59" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU59" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AV59" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="AW59" s="7" t="s">
         <v>51</v>
@@ -9144,7 +9091,7 @@
         <v>38</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D62" s="9">
         <v>3.6</v>
@@ -9153,7 +9100,7 @@
         <v>64</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>51</v>
@@ -9219,13 +9166,13 @@
         <v>52</v>
       </c>
       <c r="AK62" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AN62" s="4">
         <v>220</v>
       </c>
       <c r="AO62" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AP62" s="7" t="s">
         <v>51</v>
@@ -9237,7 +9184,7 @@
         <v>103</v>
       </c>
       <c r="AS62" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AT62" s="3" t="s">
         <v>51</v>
@@ -9246,7 +9193,7 @@
         <v>103</v>
       </c>
       <c r="AV62" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AW62" s="7" t="s">
         <v>51</v>
@@ -10082,8 +10029,6 @@
       <c r="AK69" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="AL69" s="10"/>
-      <c r="AM69" s="10"/>
       <c r="AN69" s="9">
         <v>100</v>
       </c>
@@ -10426,7 +10371,7 @@
         <v>51</v>
       </c>
       <c r="AA72" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AB72" s="5" t="b">
         <v>1</v>
@@ -10462,10 +10407,10 @@
         <v>225</v>
       </c>
       <c r="AO72" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP72" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="AP72" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="AQ72" s="3" t="s">
         <v>51</v>
@@ -10474,16 +10419,16 @@
         <v>89</v>
       </c>
       <c r="AS72" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="AT72" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU72" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="AT72" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU72" s="3" t="s">
+      <c r="AV72" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="AV72" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="AW72" s="7" t="s">
         <v>51</v>
@@ -10585,28 +10530,28 @@
         <v>5070</v>
       </c>
       <c r="AO73" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP73" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ73" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR73" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS73" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="AP73" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ73" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR73" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS73" s="3" t="s">
+      <c r="AT73" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU73" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV73" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="AT73" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU73" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AV73" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="AW73" s="7" t="s">
         <v>51</v>
@@ -10760,8 +10705,6 @@
       <c r="E75" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
       <c r="H75" s="3" t="s">
         <v>51</v>
       </c>
@@ -10833,8 +10776,6 @@
       <c r="AK75" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AL75" s="10"/>
-      <c r="AM75" s="10"/>
       <c r="AN75" s="9">
         <v>381</v>
       </c>
@@ -10842,7 +10783,7 @@
         <v>53</v>
       </c>
       <c r="AP75" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AQ75" s="3" t="s">
         <v>51</v>
@@ -11031,8 +10972,6 @@
       <c r="M77" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="N77" s="10"/>
-      <c r="O77" s="10"/>
       <c r="P77" s="3" t="s">
         <v>98</v>
       </c>
@@ -11093,8 +11032,6 @@
       <c r="AK77" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AL77" s="10"/>
-      <c r="AN77" s="10"/>
       <c r="AO77" s="6" t="s">
         <v>101</v>
       </c>
@@ -11263,7 +11200,6 @@
       <c r="C79" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D79" s="10"/>
       <c r="E79" s="3" t="s">
         <v>51</v>
       </c>
@@ -11792,7 +11728,7 @@
         <v>26</v>
       </c>
       <c r="P83" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q83" s="3" t="s">
         <v>51</v>
@@ -11819,7 +11755,7 @@
         <v>51</v>
       </c>
       <c r="AA83" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB83" s="5" t="b">
         <v>1</v>
@@ -11864,7 +11800,7 @@
         <v>68</v>
       </c>
       <c r="AP83" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ83" s="3" t="s">
         <v>51</v>
@@ -11907,8 +11843,6 @@
       <c r="E84" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10"/>
       <c r="H84" s="3" t="s">
         <v>51</v>
       </c>
@@ -11984,8 +11918,6 @@
       <c r="AK84" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AL84" s="10"/>
-      <c r="AM84" s="10"/>
       <c r="AN84" s="9">
         <v>9</v>
       </c>
@@ -11993,7 +11925,7 @@
         <v>68</v>
       </c>
       <c r="AP84" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ84" s="3" t="s">
         <v>51</v>
@@ -12115,7 +12047,7 @@
         <v>68</v>
       </c>
       <c r="AP85" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AQ85" s="3" t="s">
         <v>51</v>
@@ -12265,8 +12197,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX89">
-    <sortCondition ref="C1:C89"/>
+  <autoFilter ref="B1:B87" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX86">
+    <sortCondition ref="C1:C86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>